<commit_message>
Example input: Change Team 1 to 6 members and Team 2 to 5
</commit_message>
<xml_diff>
--- a/input/students_groups.xlsx
+++ b/input/students_groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chat/Seafile/2020 HS - HCI/Project/1 Instruction/Peer assessment/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE91E7F5-3883-FF41-9BDD-BA004F4A28F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E7E097-244F-684F-923D-6294FF8B9061}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="14260" windowHeight="17420" xr2:uid="{DE8BBC77-CF84-6749-B8DA-19EE6996D549}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,7 +469,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -509,15 +509,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
         <v>2</v>

</xml_diff>

<commit_message>
Example data: fewer rows than the template. Reduce the number of rows in the template to one.
</commit_message>
<xml_diff>
--- a/input/students_groups.xlsx
+++ b/input/students_groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chat/Seafile/2020 HS - HCI/Project/1 Instruction/Peer assessment/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E7E097-244F-684F-923D-6294FF8B9061}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE95B4EB-F101-1C48-9098-0A00CB80BD32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="14260" windowHeight="17420" xr2:uid="{DE8BBC77-CF84-6749-B8DA-19EE6996D549}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Team</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Martin</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Jill</t>
+  </si>
+  <si>
+    <t>Jane</t>
   </si>
 </sst>
 </file>
@@ -451,7 +460,7 @@
   <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,13 +565,28 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>

</xml_diff>